<commit_message>
August 6th Update with UI and API
</commit_message>
<xml_diff>
--- a/src/main/resources/TestNGXML.xlsx
+++ b/src/main/resources/TestNGXML.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29130"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D5F8E83-B98B-484F-8A3A-8788CA298034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AC6F8A2-0A02-4E16-BED0-CD9D6CBDA74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
   <si>
     <t>SuiteName</t>
   </si>
@@ -94,37 +94,70 @@
     <t>TC02_logInToECSWithInvalidID</t>
   </si>
   <si>
+    <t>Regression, Sanity</t>
+  </si>
+  <si>
+    <t>Navigate Make A Payment tests</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>TC03_navigateToMakeAPaymentPage</t>
+  </si>
+  <si>
+    <t>Navigate Auto Pay tests</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>TC04_navigateToAutoPayPage</t>
+  </si>
+  <si>
+    <t>Navigate Statement tests</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>TC05_navigateToStatementsPage</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Get Data API</t>
+  </si>
+  <si>
+    <t>tests.api.SampleAPI</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>TC01_GetSomeData</t>
+  </si>
+  <si>
+    <t>ECS_API,API</t>
+  </si>
+  <si>
+    <t>ReqRes API</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>TC02_PostSomeData</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>TC03_PutSomeData</t>
+  </si>
+  <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Regression, Sanity</t>
-  </si>
-  <si>
-    <t>Navigate Make A Payment tests</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>TC03_navigateToMakeAPaymentPage</t>
-  </si>
-  <si>
-    <t>Navigate Auto Pay tests</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>TC04_navigateToAutoPayPage</t>
-  </si>
-  <si>
-    <t>Navigate Statement tests</t>
-  </si>
-  <si>
-    <t>005</t>
-  </si>
-  <si>
-    <t>TC05_navigateToStatementsPage</t>
   </si>
 </sst>
 </file>
@@ -506,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -606,7 +639,7 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -614,19 +647,19 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -643,19 +676,19 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -664,7 +697,7 @@
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
@@ -672,19 +705,19 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -697,6 +730,93 @@
       </c>
       <c r="I6" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -804,7 +924,7 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -812,19 +932,19 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -841,19 +961,19 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -862,7 +982,7 @@
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
@@ -870,19 +990,19 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Implementation of Excel Report and Change Browser
</commit_message>
<xml_diff>
--- a/src/main/resources/TestNGXML.xlsx
+++ b/src/main/resources/TestNGXML.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29203"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AC6F8A2-0A02-4E16-BED0-CD9D6CBDA74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C562B4C7-2532-4ACA-8F5B-951609C0C200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -953,7 +953,7 @@
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Mobile Web testing for Chrome and Safari
</commit_message>
<xml_diff>
--- a/src/main/resources/TestNGXML.xlsx
+++ b/src/main/resources/TestNGXML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CFC\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B674C3C-483C-4005-8422-C1703B84E51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543068DD-CE9D-453E-B2CD-49D8A3671E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="59">
   <si>
     <t>SuiteName</t>
   </si>
@@ -174,28 +174,46 @@
     <t>tests.web.ECSAndroidScripts</t>
   </si>
   <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>ECS_TEST,IOS</t>
+  </si>
+  <si>
+    <t>tests.mobile.ECSScriptsAndroid</t>
+  </si>
+  <si>
+    <t>tests.mobile.ECSScriptsIOS</t>
+  </si>
+  <si>
+    <t>TC01_IOS_logInToECSWithValidID</t>
+  </si>
+  <si>
     <t>LogIn Android tests</t>
   </si>
   <si>
-    <t>009</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>ECS_TEST,IOS</t>
-  </si>
-  <si>
-    <t>tests.mobile.ECSScriptsAndroid</t>
-  </si>
-  <si>
-    <t>tests.mobile.ECSScriptsIOS</t>
-  </si>
-  <si>
     <t>LogIn IOS tests</t>
   </si>
   <si>
-    <t>TC01_IOS_logInToECSWithValidID</t>
+    <t>011</t>
+  </si>
+  <si>
+    <t>ECS_TEST,android_chrome</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>LogIn Mobile Chrome Testing</t>
+  </si>
+  <si>
+    <t>LogIn Mobile Safari Testing</t>
+  </si>
+  <si>
+    <t>ECS_TEST,ios_safari</t>
   </si>
 </sst>
 </file>
@@ -583,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,7 +614,7 @@
     <col min="3" max="4" width="26.81640625" customWidth="1"/>
     <col min="5" max="5" width="33.7265625" customWidth="1"/>
     <col min="6" max="6" width="21.26953125" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.81640625" customWidth="1"/>
     <col min="9" max="9" width="27.26953125" customWidth="1"/>
   </cols>
@@ -865,16 +883,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
@@ -894,30 +912,88 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" t="s">
-        <v>48</v>
-      </c>
       <c r="H11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="s">
         <v>16</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I13" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cross Browser and Allure Report Integration
</commit_message>
<xml_diff>
--- a/src/main/resources/TestNGXML.xlsx
+++ b/src/main/resources/TestNGXML.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29203"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CFC\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B674C3C-483C-4005-8422-C1703B84E51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F869C4F4-C86A-467A-8217-A9B55263940C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ECS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="54">
   <si>
     <t>SuiteName</t>
   </si>
@@ -84,33 +84,36 @@
     <t>env,browser</t>
   </si>
   <si>
+    <t>ECS_TEST,Edge</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>TC02_logInToECSWithInvalidID</t>
+  </si>
+  <si>
+    <t>Regression, Sanity</t>
+  </si>
+  <si>
+    <t>Navigate Make A Payment tests</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>TC03_navigateToMakeAPaymentPage</t>
+  </si>
+  <si>
     <t>ECS_TEST,Chrome</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>TC02_logInToECSWithInvalidID</t>
-  </si>
-  <si>
-    <t>Regression, Sanity</t>
-  </si>
-  <si>
-    <t>Navigate Make A Payment tests</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>TC03_navigateToMakeAPaymentPage</t>
-  </si>
-  <si>
     <t>Navigate Auto Pay tests</t>
   </si>
   <si>
@@ -147,6 +150,9 @@
     <t>ECS_API,API</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>ReqRes API</t>
   </si>
   <si>
@@ -162,47 +168,44 @@
     <t>TC03_PutSomeData</t>
   </si>
   <si>
-    <t>N</t>
+    <t>LogIn Android tests</t>
+  </si>
+  <si>
+    <t>tests.mobile.ECSScriptsAndroid</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>TC01_Android_logInToECSWithValidID</t>
   </si>
   <si>
     <t>ECS_TEST,Android</t>
   </si>
   <si>
-    <t>TC01_Android_logInToECSWithValidID</t>
+    <t>LogIn IOS tests</t>
+  </si>
+  <si>
+    <t>tests.mobile.ECSScriptsIOS</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>TC01_IOS_logInToECSWithValidID</t>
+  </si>
+  <si>
+    <t>ECS_TEST,IOS</t>
   </si>
   <si>
     <t>tests.web.ECSAndroidScripts</t>
-  </si>
-  <si>
-    <t>LogIn Android tests</t>
-  </si>
-  <si>
-    <t>009</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>ECS_TEST,IOS</t>
-  </si>
-  <si>
-    <t>tests.mobile.ECSScriptsAndroid</t>
-  </si>
-  <si>
-    <t>tests.mobile.ECSScriptsIOS</t>
-  </si>
-  <si>
-    <t>LogIn IOS tests</t>
-  </si>
-  <si>
-    <t>TC01_IOS_logInToECSWithValidID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,23 +588,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" customWidth="1"/>
-    <col min="2" max="2" width="27.7265625" customWidth="1"/>
-    <col min="3" max="4" width="26.81640625" customWidth="1"/>
-    <col min="5" max="5" width="33.7265625" customWidth="1"/>
-    <col min="6" max="6" width="21.26953125" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" customWidth="1"/>
-    <col min="8" max="8" width="17.81640625" customWidth="1"/>
-    <col min="9" max="9" width="27.26953125" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +634,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -654,13 +657,13 @@
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -683,13 +686,13 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -709,30 +712,30 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -741,181 +744,181 @@
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
         <v>36</v>
       </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="H9" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="I9" t="s">
         <v>40</v>
       </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
         <v>52</v>
       </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" t="s">
-        <v>48</v>
-      </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="I11" t="s">
         <v>17</v>
@@ -931,22 +934,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854EA588-8ED6-4B8C-ABB9-DBA184A95729}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="31.54296875" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -975,7 +978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -995,16 +998,16 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1024,16 +1027,16 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1056,56 +1059,56 @@
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -1114,13 +1117,13 @@
         <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1128,22 +1131,22 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>

</xml_diff>